<commit_message>
Project + Industrial Interaction Models
The project and the industrial interaction fields have been added.
The consultancy model now has a description field.
Sizes of certain fields have been updated to be more realistic.
Employee ID has been made mandatory for all records and does not allow null.
</commit_message>
<xml_diff>
--- a/Documentation/known_bugs.xlsx
+++ b/Documentation/known_bugs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anirudh\Projects\CSGT Progress Track\CSGT-Progress-Track\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4ADCDCC-CAC5-4D5B-9940-2F0440BE01E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D78D6A-A7DC-40DB-8C43-CF554A4E69AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FFA32A6B-FB61-44A5-AFB0-331A24CC6C17}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Known Bugs</t>
   </si>
@@ -130,7 +130,19 @@
     <t>Fixed by checking group variable and preventing entry to others.</t>
   </si>
   <si>
-    <t>DOI is optional and cannot be used. Hence must be checked with title.</t>
+    <t>FREND4</t>
+  </si>
+  <si>
+    <t>Add a dropdown of the titles or the primary key field when doing an update. This can help in preventing creation of a new record.</t>
+  </si>
+  <si>
+    <t>Updates can create a new record if not properly entered.</t>
+  </si>
+  <si>
+    <t>Author position is now removed hence bug fix is not required.</t>
+  </si>
+  <si>
+    <t>Report is now generated in groups hence bug fix is not required.</t>
   </si>
 </sst>
 </file>
@@ -190,12 +202,12 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -511,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92B4A9D-63F0-4D33-B77F-6A2D090FFF3D}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,30 +537,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -556,14 +568,14 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>31</v>
+      <c r="D4" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -573,7 +585,7 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -581,21 +593,24 @@
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D7" t="s">
@@ -609,10 +624,10 @@
       <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -634,7 +649,7 @@
       <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -645,8 +660,19 @@
       <c r="B11" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>